<commit_message>
Actualización automática: 2026-01-13 10:18:13
</commit_message>
<xml_diff>
--- a/Trendmicro/Salidas_Playbooks/reporte_trendmicro.xlsx
+++ b/Trendmicro/Salidas_Playbooks/reporte_trendmicro.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -435,8 +435,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="28" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="16" customWidth="1" min="5" max="5"/>
@@ -526,44 +526,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>WEB01</t>
+          <t>APP01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>vm-qa-appps-bog-01</t>
+          <t>vm-prd-appps-bog-06</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>172.25.18.227</t>
+          <t>172.25.98.111</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>No instalado</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>20.0.2</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>29810.ol8</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
       <c r="I2" t="inlineStr">
         <is>
           <t>1.2.0.956</t>
@@ -581,7 +581,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -598,44 +598,44 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>WEB02</t>
+          <t>APP02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vm-qa-appps-bog-02</t>
+          <t>vm-prd-appps-bog-07</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>172.25.18.82</t>
+          <t>172.25.96.193</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>No instalado</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>20.0.2</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>29810.ol8</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>1.2.0.956</t>
@@ -653,7 +653,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -670,44 +670,44 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>APP01</t>
+          <t>BATCH01</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>vm-qa-appps-bog-03</t>
+          <t>vm-prd-appps-bog-08</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>172.25.18.232</t>
+          <t>172.25.96.96</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>No instalado</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>20.0.2</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>29810.ol8</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
       <c r="I4" t="inlineStr">
         <is>
           <t>1.2.0.956</t>
@@ -725,7 +725,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -742,44 +742,44 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>APP02</t>
+          <t>BATCH02</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>vm-qa-appps-bog-04</t>
+          <t>vm-prd-appps-bog-09</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>172.25.17.123</t>
+          <t>172.25.99.10</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>No instalado</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>20.0.2</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>29810.ol8</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>1.2.0.956</t>
@@ -797,7 +797,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -814,17 +814,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BATCH01</t>
+          <t>WS01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>vm-qa-appps-bog-05</t>
+          <t>vm-prd-appps-bog-01-950287</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>172.25.17.218</t>
+          <t>172.25.97.44</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -886,27 +886,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BATCH02</t>
+          <t>WS02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>vm-qa-appps-bog-06</t>
+          <t>vm-prd-appps-bog-02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>172.25.16.248</t>
+          <t>172.25.97.201</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>No instalado</t>
+          <t>20.0.2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>No instalado</t>
+          <t>29810.ol8</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -921,17 +921,17 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>No instalado</t>
+          <t>1.2.0.1253</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1.2.0.956</t>
+          <t>1.2.0.1253</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -958,44 +958,44 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>VM-QA-APPPS-BOG-08</t>
+          <t>BATCH03</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>vm-qa-appps-bog-08</t>
+          <t>vm-prd-appps-bog-10</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>172.25.19.107</t>
+          <t>172.25.99.176</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
           <t>No instalado</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>20.0.2</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>29810.ol8</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
       <c r="I8" t="inlineStr">
         <is>
           <t>1.2.0.956</t>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1030,44 +1030,44 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>VM-QA-APPPS-BOG-09</t>
+          <t>BATCH04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>vm-qa-appps-bog-09</t>
+          <t>vm-prd-appps-bog-11</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>172.25.18.253</t>
+          <t>172.25.96.209</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
           <t>No instalado</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>20.0.2</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>29810.ol8</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
       <c r="I9" t="inlineStr">
         <is>
           <t>1.2.0.956</t>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1102,70 +1102,142 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DESA01</t>
+          <t>MASTER01</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>vm-dev-ps-app-bog-01</t>
+          <t>vm-prd-appps-bog-12</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>172.25.35.72</t>
+          <t>172.25.97.108</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>29760.ol8</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>29760.ol8</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1.2.0.1102</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1.2.0.1102</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="N10" s="2" t="inlineStr">
+        <is>
+          <t>REVISAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MASTER02</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>vm-prd-appps-bog-13</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>172.25.98.228</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>20.0.2</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>29810.ol8</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>No instalado</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>20.0.2</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>29810.ol8</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>No instalado</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>1.2.0.956</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>no activo</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>no activo</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="N10" s="2" t="inlineStr">
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="N11" s="2" t="inlineStr">
         <is>
           <t>REVISAR</t>
         </is>

</xml_diff>

<commit_message>
Actualización automática: 2026-02-18 08:19:23
</commit_message>
<xml_diff>
--- a/Trendmicro/Salidas_Playbooks/reporte_trendmicro.xlsx
+++ b/Trendmicro/Salidas_Playbooks/reporte_trendmicro.xlsx
@@ -435,9 +435,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
-    <col width="21" customWidth="1" min="2" max="2"/>
-    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="16" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
@@ -526,17 +526,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VM-EU2-APPDRU03-RST</t>
+          <t>GEOJENKINS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VM-EU2-APPDRU03-RST</t>
+          <t>geojenkins</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10.0.16.149</t>
+          <t>10.181.4.105</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -561,22 +561,22 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1.2.0.1253</t>
+          <t>No instalado</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1.2.0.1253</t>
+          <t>1.2.0.956</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>desconocido</t>
+          <t>inactive</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">

</xml_diff>

<commit_message>
Actualización automática: 2026-02-24 09:59:58
</commit_message>
<xml_diff>
--- a/Trendmicro/Salidas_Playbooks/reporte_trendmicro.xlsx
+++ b/Trendmicro/Salidas_Playbooks/reporte_trendmicro.xlsx
@@ -435,8 +435,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="16" customWidth="1" min="5" max="5"/>
@@ -526,47 +526,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GEOJENKINS</t>
+          <t>mongodb_qa_micro01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>geojenkins</t>
+          <t>mongodb_qa_micro01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10.181.4.105</t>
+          <t>10.181.34.51</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>No instalado</t>
+          <t>20.0.3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>No instalado</t>
+          <t>860.ol8</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>No instalado</t>
+          <t>20.0.3</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>No instalado</t>
+          <t>860.ol8</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>No instalado</t>
+          <t>1.2.0.1253</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1.2.0.956</t>
+          <t>1.2.0.1253</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -576,17 +576,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>inactive</t>
+          <t>active</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>no activo</t>
+          <t>active</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>desconocido</t>
+          <t>active</t>
         </is>
       </c>
       <c r="N2" s="2" t="inlineStr">

</xml_diff>